<commit_message>
Update URLs and email addresses (#265)
Amend URLs to the new domain countermetrics.org. Change all emails to code@countermetrics.org to ensure continuity. Change role description where relevant.
</commit_message>
<xml_diff>
--- a/source/_static/report/DRD1_sample_r51.xlsx
+++ b/source/_static/report/DRD1_sample_r51.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\COUNTER\Release 5.1\Sample reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58A4A047-993F-4919-88E3-96D3303CF47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DD7AA6-D6D9-4AE6-AD00-52ED77D4841A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{621E1D3D-4D00-4D63-B418-B55B9B62E580}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{621E1D3D-4D00-4D63-B418-B55B9B62E580}"/>
   </bookViews>
   <sheets>
     <sheet name="DRD1_sample_r51" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>Registry_Record</t>
   </si>
   <si>
-    <t>https://registry.projectcounter.org/platform/99999999-9999-9999-9999-999999999999</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -951,6 +948,9 @@
   </si>
   <si>
     <t>1393</t>
+  </si>
+  <si>
+    <t>https://registry.countermetrics.org/platform/99999999-9999-9999-9999-999999999999</t>
   </si>
 </sst>
 </file>
@@ -1019,9 +1019,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1059,7 +1059,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1165,7 +1165,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1307,7 +1307,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1709,7 +1709,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>304</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1766,61 +1766,61 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -1832,61 +1832,61 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -1898,61 +1898,61 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -1964,61 +1964,61 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -2030,61 +2030,61 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -2096,61 +2096,61 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -2162,61 +2162,61 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -2228,61 +2228,61 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="R22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -2294,61 +2294,61 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
@@ -2360,61 +2360,61 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
@@ -2426,61 +2426,61 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
@@ -2492,61 +2492,61 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="R26" s="1" t="s">
+      <c r="S26" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -2558,61 +2558,61 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="R27" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -2624,61 +2624,61 @@
     </row>
     <row r="28" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E28" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="R28" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
@@ -2690,61 +2690,61 @@
     </row>
     <row r="29" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="R29" s="1" t="s">
+      <c r="S29" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -2756,61 +2756,61 @@
     </row>
     <row r="30" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="R30" s="1" t="s">
+      <c r="S30" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
@@ -2822,61 +2822,61 @@
     </row>
     <row r="31" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="S31" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -2888,61 +2888,61 @@
     </row>
     <row r="32" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="S32" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -2954,61 +2954,61 @@
     </row>
     <row r="33" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="R33" s="1" t="s">
+      <c r="S33" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
@@ -3020,61 +3020,61 @@
     </row>
     <row r="34" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="R34" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
@@ -30078,7 +30078,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{87E624EF-001C-42DE-BD72-939AE936C82B}"/>
+    <hyperlink ref="B13" r:id="rId1" display="https://registry.projectcounter.org/platform/99999999-9999-9999-9999-999999999999" xr:uid="{87E624EF-001C-42DE-BD72-939AE936C82B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>